<commit_message>
updated the estimated storage charges
</commit_message>
<xml_diff>
--- a/aro 4 calculator.xlsx
+++ b/aro 4 calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydodg\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D1A6B6-B575-417A-994A-24B673D1A4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D34DA94-174B-4537-BF1C-79B84214699A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9EB61050-8035-41A8-8F43-766506FE4D36}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="1" xr2:uid="{9EB61050-8035-41A8-8F43-766506FE4D36}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="3" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>Annualized</t>
-  </si>
-  <si>
     <t>Core Count</t>
   </si>
   <si>
@@ -158,36 +155,6 @@
   </si>
   <si>
     <t>Azure Credit</t>
-  </si>
-  <si>
-    <t>Cluster App Node Azure Charge</t>
-  </si>
-  <si>
-    <t>Cluster App Node OpenShift Charge</t>
-  </si>
-  <si>
-    <t>Cluster Master Node Azure Charge</t>
-  </si>
-  <si>
-    <t>Cluster Azure Storage Charge Estimate</t>
-  </si>
-  <si>
-    <t>Cluster Azure Load Balancer Charge Estimate</t>
-  </si>
-  <si>
-    <t>Cluster Azure Other 1 Charge Estimate</t>
-  </si>
-  <si>
-    <t>Cluster Azure Other 2 Charge Estimate</t>
-  </si>
-  <si>
-    <t>Gross Cluster Azure Charge</t>
-  </si>
-  <si>
-    <t>Gross Cluster OpenShift Charge</t>
-  </si>
-  <si>
-    <t>Gross Cluster Charge Total</t>
   </si>
   <si>
     <t>https://azure.microsoft.com/pricing/calculator/</t>
@@ -277,6 +244,39 @@
   </si>
   <si>
     <t>&lt;-- Azure Credit ROI</t>
+  </si>
+  <si>
+    <t>Gross Azure Cluster Charge</t>
+  </si>
+  <si>
+    <t>Gross OpenShift Cluster Licensing Charge</t>
+  </si>
+  <si>
+    <t>Cluster Azure Other 2 Charge</t>
+  </si>
+  <si>
+    <t>Cluster Azure Other 1 Charge</t>
+  </si>
+  <si>
+    <t>Cluster Azure Load Balancer Charge</t>
+  </si>
+  <si>
+    <t>Cluster Azure Storage (~40% of Compute)</t>
+  </si>
+  <si>
+    <t>Cluster Azure Master Node Compute</t>
+  </si>
+  <si>
+    <t>Cluster Azure App Node Compute</t>
+  </si>
+  <si>
+    <t>Cluster OpenShift App Node Licensing</t>
+  </si>
+  <si>
+    <t>Gross Total Cluster Charge</t>
+  </si>
+  <si>
+    <t>Annual</t>
   </si>
 </sst>
 </file>
@@ -757,98 +757,98 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -866,12 +866,12 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="13" width="10.88671875" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
     <col min="15" max="15" width="10.109375" customWidth="1"/>
@@ -919,7 +919,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1641,7 +1641,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <f>B15*VLOOKUP(B16,SKU_CHARGES!$A$2:$F$13,6,FALSE)+B3*VLOOKUP(B4,SKU_CHARGES!$A$2:$F$13,6,FALSE)+B7*VLOOKUP(B8,SKU_CHARGES!$A$2:$F$13,6,FALSE)+B11*VLOOKUP(B12,SKU_CHARGES!$A$2:$F$13,6,FALSE)</f>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18:M18" si="1">SUM(B13,B9,B5)</f>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19:M19" si="2">SUM(B14,B10,B6,)</f>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2">
         <f>B2*B15*VLOOKUP(B16,SKU_CHARGES!$A$2:$E$13,5,FALSE)</f>
@@ -1866,52 +1866,64 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2">
-        <v>57.24</v>
+        <f>40%*SUM(B19:B20)</f>
+        <v>504.57600000000002</v>
       </c>
       <c r="C21" s="2">
-        <v>57.24</v>
+        <f t="shared" ref="C21:M21" si="3">40%*SUM(C19:C20)</f>
+        <v>504.57600000000002</v>
       </c>
       <c r="D21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="E21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="F21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="G21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="H21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="I21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="J21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="K21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="L21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="M21" s="2">
-        <v>57.24</v>
+        <f t="shared" si="3"/>
+        <v>504.57600000000002</v>
       </c>
       <c r="N21" s="6">
-        <f t="shared" ref="N21:N27" si="3">SUM(B21:M21)</f>
-        <v>686.88</v>
+        <f t="shared" ref="N21:N27" si="4">SUM(B21:M21)</f>
+        <v>6054.9120000000003</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1950,13 +1962,13 @@
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1995,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="N23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -2040,187 +2052,187 @@
         <v>0</v>
       </c>
       <c r="N24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B25" s="1">
         <f>SUM(B19:B24)</f>
-        <v>1318.68</v>
+        <v>1766.0160000000001</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:M25" si="4">SUM(C19:C24)</f>
-        <v>1318.68</v>
+        <f t="shared" ref="C25:M25" si="5">SUM(C19:C24)</f>
+        <v>1766.0160000000001</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="4"/>
-        <v>1318.68</v>
+        <f t="shared" si="5"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="N25" s="6">
         <f>SUM(B25:M25)</f>
-        <v>15824.160000000002</v>
+        <v>21192.191999999999</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2">
         <f>B18</f>
         <v>1666.59</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" ref="C26:M26" si="5">C18</f>
+        <f t="shared" ref="C26:M26" si="6">C18</f>
         <v>1666.59</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1666.59</v>
       </c>
       <c r="N26" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19999.079999999998</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2">
         <f>SUM(B25:B26)</f>
-        <v>2985.27</v>
+        <v>3432.6059999999998</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" ref="C27:M27" si="6">SUM(C25:C26)</f>
-        <v>2985.27</v>
+        <f t="shared" ref="C27:M27" si="7">SUM(C25:C26)</f>
+        <v>3432.6059999999998</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="6"/>
-        <v>2985.27</v>
+        <f t="shared" si="7"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="N27" s="8">
-        <f t="shared" si="3"/>
-        <v>35823.24</v>
+        <f t="shared" si="4"/>
+        <v>41191.271999999997</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C28" s="11">
         <v>0</v>
@@ -2257,19 +2269,19 @@
       </c>
       <c r="N28" s="6">
         <f>SUM(B28:M28)</f>
-        <v>1000</v>
-      </c>
-      <c r="O28" s="16">
+        <v>0</v>
+      </c>
+      <c r="O28" s="16" t="str">
         <f>IFERROR(ABS(N25)/ABS(N28), "N/A")</f>
-        <v>15.824160000000001</v>
+        <v>N/A</v>
       </c>
       <c r="P28" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B29" s="12">
         <v>0</v>
@@ -2310,214 +2322,214 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="L30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="M30" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2">
         <f>B25*(1-B29)*(1-B30)</f>
-        <v>1120.8779999999999</v>
+        <v>1766.0160000000001</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" ref="C31:M31" si="7">C25*(1-C29)*(1-C30)</f>
-        <v>1120.8779999999999</v>
+        <f t="shared" ref="C31:M31" si="8">C25*(1-C29)*(1-C30)</f>
+        <v>1766.0160000000001</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="7"/>
-        <v>1120.8779999999999</v>
+        <f t="shared" si="8"/>
+        <v>1766.0160000000001</v>
       </c>
       <c r="N31" s="6">
         <f>SUM(B31:M31)</f>
-        <v>13450.536000000002</v>
+        <v>21192.191999999999</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2">
         <f>B18*(1-B29)*(1-B30)</f>
-        <v>1416.6015</v>
+        <v>1666.59</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" ref="C32:M32" si="8">C18*(1-C29)*(1-C30)</f>
-        <v>1416.6015</v>
+        <f t="shared" ref="C32:M32" si="9">C18*(1-C29)*(1-C30)</f>
+        <v>1666.59</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="8"/>
-        <v>1416.6015</v>
+        <f t="shared" si="9"/>
+        <v>1666.59</v>
       </c>
       <c r="N32" s="7">
         <f>SUM(B32:M32)</f>
-        <v>16999.218000000004</v>
+        <v>19999.079999999998</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2">
         <f>SUM(B31:B32)</f>
-        <v>2537.4794999999999</v>
+        <v>3432.6059999999998</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" ref="C33:M33" si="9">SUM(C31:C32)</f>
-        <v>2537.4794999999999</v>
+        <f t="shared" ref="C33:M33" si="10">SUM(C31:C32)</f>
+        <v>3432.6059999999998</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="9"/>
-        <v>2537.4794999999999</v>
+        <f t="shared" si="10"/>
+        <v>3432.6059999999998</v>
       </c>
       <c r="N33" s="8">
         <f>SUM(B33:M33)</f>
-        <v>30449.754000000004</v>
+        <v>41191.271999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2543,7 @@
           <x14:formula1>
             <xm:f>SKU_CHARGES!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 C4:M4 B8:M8 B12:M12 B16:M16</xm:sqref>
+          <xm:sqref>B4:M4 B8:M8 B12:M12 B16:M16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2573,7 +2585,7 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>